<commit_message>
Before trying to make the corr matrix in a new way
</commit_message>
<xml_diff>
--- a/corr.xlsx
+++ b/corr.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="106">
   <si>
     <t>1. Страна</t>
   </si>
@@ -1082,10 +1082,10 @@
   <dimension ref="A1:CA79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="BJ57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CA78" sqref="CA78"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +1094,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f ca="1">MDETERM($D$3:INDIRECT("R"&amp;$B$1+2&amp;"C"&amp;$B$1+3,FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -1225,6 +1232,10 @@
       </c>
     </row>
     <row r="2" spans="1:79" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">INDIRECT("R"&amp;$B$1+3&amp;"C"&amp;$B$1+4,FALSE)</f>
+        <v>1</v>
+      </c>
       <c r="D2" t="s">
         <v>37</v>
       </c>
@@ -1465,18 +1476,30 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I3">
+        <v>-1</v>
+      </c>
+      <c r="J3">
+        <v>-0.95</v>
+      </c>
+      <c r="K3">
+        <v>-0.9</v>
+      </c>
+      <c r="L3">
+        <v>0.8</v>
+      </c>
+      <c r="M3">
         <v>0</v>
       </c>
     </row>
@@ -1485,21 +1508,33 @@
         <v>38</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <v>0.95</v>
+      </c>
+      <c r="K4">
+        <v>-0.9</v>
+      </c>
+      <c r="L4">
+        <v>-0.95</v>
+      </c>
+      <c r="M4">
         <v>0</v>
       </c>
     </row>
@@ -1508,22 +1543,34 @@
         <v>39</v>
       </c>
       <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>-0.95</v>
+      </c>
+      <c r="K5">
+        <v>-0.9</v>
+      </c>
+      <c r="L5">
+        <v>0.7</v>
+      </c>
+      <c r="M5">
         <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.25">
@@ -1537,18 +1584,30 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6">
+        <v>-1</v>
+      </c>
+      <c r="J6">
+        <v>-0.95</v>
+      </c>
+      <c r="K6">
+        <v>-0.9</v>
+      </c>
+      <c r="L6">
+        <v>0.8</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
     </row>
@@ -1557,21 +1616,33 @@
         <v>41</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <v>0.95</v>
+      </c>
+      <c r="K7">
+        <v>-0.9</v>
+      </c>
+      <c r="L7">
+        <v>-0.95</v>
+      </c>
+      <c r="M7">
         <v>0</v>
       </c>
     </row>
@@ -1580,22 +1651,34 @@
         <v>82</v>
       </c>
       <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>-0.95</v>
+      </c>
+      <c r="K8">
+        <v>-0.9</v>
+      </c>
+      <c r="L8">
+        <v>0.7</v>
+      </c>
+      <c r="M8">
         <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:79" x14ac:dyDescent="0.25">
@@ -1608,53 +1691,137 @@
       <c r="C9" t="s">
         <v>83</v>
       </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>87</v>
+      <c r="D9">
+        <v>-0.95</v>
+      </c>
+      <c r="E9">
+        <v>0.95</v>
+      </c>
+      <c r="F9">
+        <v>-0.95</v>
+      </c>
+      <c r="G9">
+        <v>-0.95</v>
+      </c>
+      <c r="H9">
+        <v>0.95</v>
+      </c>
+      <c r="I9">
+        <v>-0.95</v>
       </c>
       <c r="J9">
         <v>1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <v>-1</v>
+      </c>
+      <c r="M9">
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>84</v>
       </c>
+      <c r="D10">
+        <v>-0.9</v>
+      </c>
+      <c r="E10">
+        <v>-0.9</v>
+      </c>
+      <c r="F10">
+        <v>-0.9</v>
+      </c>
+      <c r="G10">
+        <v>-0.9</v>
+      </c>
+      <c r="H10">
+        <v>-0.9</v>
+      </c>
+      <c r="I10">
+        <v>-0.9</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
       <c r="K10">
         <v>1</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" t="s">
-        <v>86</v>
+      <c r="D11">
+        <v>0.8</v>
+      </c>
+      <c r="E11">
+        <v>-0.95</v>
+      </c>
+      <c r="F11">
+        <v>0.7</v>
+      </c>
+      <c r="G11">
+        <v>0.8</v>
+      </c>
+      <c r="H11">
+        <v>-0.95</v>
+      </c>
+      <c r="I11">
+        <v>0.7</v>
+      </c>
+      <c r="J11">
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
       </c>
       <c r="L11">
         <v>1</v>
+      </c>
+      <c r="M11">
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>77</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>-1</v>
+      </c>
+      <c r="K12">
+        <v>-1</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
       </c>
       <c r="M12">
         <v>1</v>

</xml_diff>